<commit_message>
Updated the truth table
</commit_message>
<xml_diff>
--- a/Arm-y_Hard_Truth_Table.xlsx
+++ b/Arm-y_Hard_Truth_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kojo\Documents\GitHub\ARM-y_Hard-Coding-Competion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EDED69-F694-4DF6-BC98-6D43F3AB6F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450E4F64-5568-4244-93CE-15070DE97E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{760FCC2E-0B54-40DF-A8E6-BF07013B5595}"/>
   </bookViews>
@@ -420,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AC87B1D-AD20-4646-82B0-4CF01A7B9822}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -953,7 +953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -972,8 +972,23 @@
       <c r="F18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -992,8 +1007,23 @@
       <c r="F19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
@@ -1012,8 +1042,23 @@
       <c r="F20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -1032,8 +1077,23 @@
       <c r="F21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0</v>
       </c>
@@ -1052,8 +1112,23 @@
       <c r="F22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
@@ -1072,8 +1147,23 @@
       <c r="F23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0</v>
       </c>
@@ -1090,6 +1180,98 @@
         <v>0</v>
       </c>
       <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
         <v>1</v>
       </c>
     </row>

</xml_diff>